<commit_message>
Cleaning up before final submission
Moved lots of file to ForLater folder. See the ReadMe.txt file there for
further work that would be part of my PhD thesis.
</commit_message>
<xml_diff>
--- a/Code/R/Data.xlsx
+++ b/Code/R/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Model File</t>
   </si>
@@ -69,15 +69,9 @@
     <t>SearchType</t>
   </si>
   <si>
-    <t>2000-2500/10</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>PerfSerach_Classification_TenfoldCV_SMOTE217</t>
-  </si>
-  <si>
     <t>1500-2800/50</t>
   </si>
   <si>
@@ -90,8 +84,19 @@
     <t>na</t>
   </si>
   <si>
-    <t>PerfSearch_Classification_TenfoldCV_WEKA_SMOTE217_NormFeaturized + PerfSearch_Classification_IT_WEKA_SMOTE217_NormFeaturized +
-PerfSearch_Classification_JackKnifeCV_WEKA_SMOTE217_NormFeaturized</t>
+    <t>PerfSearch_Classification_TenfoldCV_WEKA_SMOTE217</t>
+  </si>
+  <si>
+    <t>Learning Type</t>
+  </si>
+  <si>
+    <t>SVM Class.</t>
+  </si>
+  <si>
+    <t>PerfSearch_Regression_TenfoldCV_WEKA_SMOTE217</t>
+  </si>
+  <si>
+    <t>SVM Regress.</t>
   </si>
 </sst>
 </file>
@@ -438,21 +443,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="67.28515625" customWidth="1"/>
-    <col min="2" max="5" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="2" max="6" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1">
+    <row r="1" spans="1:18" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,221 +465,212 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>19</v>
+    <row r="2" spans="1:18" ht="49.5" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2">
-        <v>2010</v>
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>0.03</v>
+        <v>2800</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0.94930879999999995</v>
+      </c>
+      <c r="H2">
+        <v>0.94009220000000004</v>
+      </c>
+      <c r="I2">
+        <v>0.95852530000000002</v>
       </c>
       <c r="J2">
-        <v>94.700460000000007</v>
+        <v>0.89877019999999996</v>
       </c>
       <c r="K2">
-        <v>97.695849999999993</v>
+        <v>0.94700460829493105</v>
       </c>
       <c r="L2">
-        <v>91.705070000000006</v>
+        <v>0.93548387096774199</v>
       </c>
       <c r="M2">
-        <v>0.9</v>
+        <v>0.95852534562212</v>
+      </c>
+      <c r="N2">
+        <v>0.89424663014522598</v>
+      </c>
+      <c r="O2">
+        <v>0.9375</v>
+      </c>
+      <c r="P2">
+        <v>0.98039220000000005</v>
+      </c>
+      <c r="Q2">
+        <v>0.76923079999999999</v>
+      </c>
+      <c r="R2">
+        <v>0.79940219999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="49.5" customHeight="1">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>94.9</v>
+      </c>
+      <c r="H5">
+        <v>97.2</v>
+      </c>
+      <c r="I5">
+        <v>92.6</v>
+      </c>
+      <c r="J5">
+        <v>0.9</v>
+      </c>
+      <c r="K5">
+        <v>94.9</v>
+      </c>
+      <c r="L5">
+        <v>97.2</v>
+      </c>
+      <c r="M5">
+        <v>92.6</v>
+      </c>
+      <c r="N5">
+        <v>0.9</v>
+      </c>
+      <c r="O5">
+        <v>94.8</v>
+      </c>
+      <c r="P5">
+        <v>94</v>
+      </c>
+      <c r="Q5">
+        <v>93.9</v>
+      </c>
+      <c r="R5">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
         <v>20</v>
-      </c>
-      <c r="D3">
-        <v>2800</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>0.94930875599999998</v>
-      </c>
-      <c r="G3">
-        <v>0.94470046100000005</v>
-      </c>
-      <c r="H3">
-        <v>0.95391705100000002</v>
-      </c>
-      <c r="I3">
-        <v>0.89865568100000004</v>
-      </c>
-      <c r="J3">
-        <v>0.94700460829493105</v>
-      </c>
-      <c r="K3">
-        <v>0.93548387096774199</v>
-      </c>
-      <c r="L3">
-        <v>0.95852534562212</v>
-      </c>
-      <c r="M3">
-        <v>0.89424663014522598</v>
-      </c>
-      <c r="N3">
-        <v>0.9375</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>0.69230769230769196</v>
-      </c>
-      <c r="Q3">
-        <v>0.80122284163523605</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="F6">
-        <v>94.9</v>
+      <c r="F6" t="s">
+        <v>21</v>
       </c>
       <c r="G6">
-        <v>97.2</v>
+        <v>88.5</v>
       </c>
       <c r="H6">
-        <v>92.6</v>
+        <v>88.9</v>
       </c>
       <c r="I6">
-        <v>0.9</v>
+        <v>88</v>
       </c>
       <c r="J6">
-        <v>94.9</v>
+        <v>0.76</v>
       </c>
       <c r="K6">
-        <v>97.2</v>
+        <v>90.1</v>
       </c>
       <c r="L6">
-        <v>92.6</v>
+        <v>90.8</v>
       </c>
       <c r="M6">
-        <v>0.9</v>
+        <v>89.4</v>
       </c>
       <c r="N6">
-        <v>94.8</v>
+        <v>0.8</v>
       </c>
       <c r="O6">
-        <v>94</v>
+        <v>93.8</v>
       </c>
       <c r="P6">
-        <v>93.9</v>
+        <v>92.3</v>
       </c>
       <c r="Q6">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>88.5</v>
-      </c>
-      <c r="G7">
-        <v>88.9</v>
-      </c>
-      <c r="H7">
-        <v>88</v>
-      </c>
-      <c r="I7">
-        <v>0.76</v>
-      </c>
-      <c r="J7">
-        <v>90.1</v>
-      </c>
-      <c r="K7">
-        <v>90.8</v>
-      </c>
-      <c r="L7">
-        <v>89.4</v>
-      </c>
-      <c r="M7">
-        <v>0.8</v>
-      </c>
-      <c r="N7">
-        <v>93.8</v>
-      </c>
-      <c r="O7">
-        <v>92.3</v>
-      </c>
-      <c r="P7">
         <v>94.1</v>
       </c>
-      <c r="Q7">
+      <c r="R6">
         <v>0.82</v>
       </c>
     </row>

</xml_diff>